<commit_message>
Document sprint 11 #105
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\Dropbox\Carpetas_compartidas\Universidad\TFG\go-bees\docs\md\anexos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\Dropbox\Carpetas_compartidas\Universidad\TFG\go-bees\docs\rst\anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Sprint 11</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -355,162 +358,326 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="154">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="168">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2154,8 +2321,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="153" headerRowBorderDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="167" headerRowBorderDxfId="166">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="165" totalsRowDxfId="164"/>
+    <tableColumn id="2" name="Min." dataDxfId="163" totalsRowDxfId="162"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="161" totalsRowDxfId="160"/>
+    <tableColumn id="4" name="Total" dataDxfId="159" totalsRowDxfId="158"/>
+    <tableColumn id="5" name="Real" dataDxfId="157" totalsRowDxfId="156"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="155" totalsRowDxfId="154"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2175,39 +2409,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2227,9 +2431,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2249,16 +2453,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
     <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
@@ -2271,9 +2468,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
     <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
@@ -2286,9 +2483,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
     <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
@@ -2301,9 +2498,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
     <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
@@ -2316,9 +2513,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
     <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
@@ -2326,21 +2523,6 @@
     <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
     <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2609,10 +2791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G152"/>
+  <dimension ref="B1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="G152" sqref="G152"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,22 +2805,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -2861,22 +3043,22 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -3095,22 +3277,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
@@ -3329,22 +3511,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -3563,22 +3745,22 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
@@ -3797,22 +3979,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="22"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
     </row>
     <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
@@ -4031,22 +4213,22 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
     </row>
     <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="22"/>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
     </row>
     <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
@@ -4265,22 +4447,22 @@
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
-      <c r="E99" s="21"/>
-      <c r="F99" s="21"/>
-      <c r="G99" s="21"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="22"/>
-      <c r="C100" s="22"/>
-      <c r="D100" s="22"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -4499,22 +4681,22 @@
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="21" t="s">
+      <c r="B113" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="21"/>
-      <c r="D113" s="21"/>
-      <c r="E113" s="21"/>
-      <c r="F113" s="21"/>
-      <c r="G113" s="21"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
+      <c r="G113" s="22"/>
     </row>
     <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="22"/>
-      <c r="C114" s="22"/>
-      <c r="D114" s="22"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="22"/>
-      <c r="G114" s="22"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
     </row>
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
@@ -4733,22 +4915,22 @@
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="21" t="s">
+      <c r="B127" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="21"/>
-      <c r="D127" s="21"/>
-      <c r="E127" s="21"/>
-      <c r="F127" s="21"/>
-      <c r="G127" s="21"/>
+      <c r="C127" s="22"/>
+      <c r="D127" s="22"/>
+      <c r="E127" s="22"/>
+      <c r="F127" s="22"/>
+      <c r="G127" s="22"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="22"/>
-      <c r="C128" s="22"/>
-      <c r="D128" s="22"/>
-      <c r="E128" s="22"/>
-      <c r="F128" s="22"/>
-      <c r="G128" s="22"/>
+      <c r="B128" s="23"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="23"/>
+      <c r="G128" s="23"/>
     </row>
     <row r="129" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
@@ -4967,22 +5149,22 @@
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="21" t="s">
+      <c r="B141" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C141" s="21"/>
-      <c r="D141" s="21"/>
-      <c r="E141" s="21"/>
-      <c r="F141" s="21"/>
-      <c r="G141" s="21"/>
+      <c r="C141" s="22"/>
+      <c r="D141" s="22"/>
+      <c r="E141" s="22"/>
+      <c r="F141" s="22"/>
+      <c r="G141" s="22"/>
     </row>
     <row r="142" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="22"/>
-      <c r="C142" s="22"/>
-      <c r="D142" s="22"/>
-      <c r="E142" s="22"/>
-      <c r="F142" s="22"/>
-      <c r="G142" s="22"/>
+      <c r="B142" s="23"/>
+      <c r="C142" s="23"/>
+      <c r="D142" s="23"/>
+      <c r="E142" s="23"/>
+      <c r="F142" s="23"/>
+      <c r="G142" s="23"/>
     </row>
     <row r="143" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="5" t="s">
@@ -5195,13 +5377,248 @@
       <c r="F152" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G152" s="23">
+      <c r="G152" s="21">
         <f>SUM(G144:G151)/60</f>
         <v>39.25</v>
       </c>
     </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B155" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C155" s="22"/>
+      <c r="D155" s="22"/>
+      <c r="E155" s="22"/>
+      <c r="F155" s="22"/>
+      <c r="G155" s="22"/>
+    </row>
+    <row r="156" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="23"/>
+      <c r="C156" s="23"/>
+      <c r="D156" s="23"/>
+      <c r="E156" s="23"/>
+      <c r="F156" s="23"/>
+      <c r="G156" s="23"/>
+    </row>
+    <row r="157" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G157" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B158" s="14">
+        <v>1</v>
+      </c>
+      <c r="C158" s="8">
+        <v>15</v>
+      </c>
+      <c r="D158" s="7">
+        <v>1</v>
+      </c>
+      <c r="E158" s="8">
+        <f>D158*C158</f>
+        <v>15</v>
+      </c>
+      <c r="F158" s="11">
+        <v>1</v>
+      </c>
+      <c r="G158" s="18">
+        <f>F158*C158</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B159" s="15">
+        <v>2</v>
+      </c>
+      <c r="C159" s="10">
+        <v>45</v>
+      </c>
+      <c r="D159" s="9">
+        <v>2</v>
+      </c>
+      <c r="E159" s="10">
+        <f t="shared" ref="E159:E165" si="22">D159*C159</f>
+        <v>90</v>
+      </c>
+      <c r="F159" s="12">
+        <v>1</v>
+      </c>
+      <c r="G159" s="19">
+        <f t="shared" ref="G159:G165" si="23">F159*C159</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B160" s="15">
+        <v>3</v>
+      </c>
+      <c r="C160" s="10">
+        <v>120</v>
+      </c>
+      <c r="D160" s="9">
+        <v>1</v>
+      </c>
+      <c r="E160" s="10">
+        <f t="shared" si="22"/>
+        <v>120</v>
+      </c>
+      <c r="F160" s="12">
+        <v>2</v>
+      </c>
+      <c r="G160" s="19">
+        <f t="shared" si="23"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B161" s="15">
+        <v>5</v>
+      </c>
+      <c r="C161" s="10">
+        <v>300</v>
+      </c>
+      <c r="D161" s="9">
+        <v>2</v>
+      </c>
+      <c r="E161" s="10">
+        <f t="shared" si="22"/>
+        <v>600</v>
+      </c>
+      <c r="F161" s="12">
+        <v>1</v>
+      </c>
+      <c r="G161" s="19">
+        <f t="shared" si="23"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B162" s="15">
+        <v>8</v>
+      </c>
+      <c r="C162" s="10">
+        <v>720</v>
+      </c>
+      <c r="D162" s="9">
+        <v>1</v>
+      </c>
+      <c r="E162" s="10">
+        <f t="shared" si="22"/>
+        <v>720</v>
+      </c>
+      <c r="F162" s="12">
+        <v>2</v>
+      </c>
+      <c r="G162" s="19">
+        <f t="shared" si="23"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B163" s="15">
+        <v>13</v>
+      </c>
+      <c r="C163" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D163" s="9">
+        <v>0</v>
+      </c>
+      <c r="E163" s="10">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F163" s="12">
+        <v>0</v>
+      </c>
+      <c r="G163" s="19">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B164" s="15">
+        <v>21</v>
+      </c>
+      <c r="C164" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D164" s="9">
+        <v>0</v>
+      </c>
+      <c r="E164" s="10">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F164" s="12">
+        <v>0</v>
+      </c>
+      <c r="G164" s="19">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="15">
+        <v>40</v>
+      </c>
+      <c r="C165" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D165" s="9">
+        <v>0</v>
+      </c>
+      <c r="E165" s="10">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F165" s="12">
+        <v>0</v>
+      </c>
+      <c r="G165" s="20">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="3"/>
+      <c r="C166" s="16"/>
+      <c r="D166" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E166" s="24">
+        <f>SUM(E158:E165)/60</f>
+        <v>25.75</v>
+      </c>
+      <c r="F166" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G166" s="21">
+        <f>SUM(G158:G165)/60</f>
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="B155:G156"/>
     <mergeCell ref="B141:G142"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B15:G16"/>
@@ -5216,7 +5633,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="11">
+  <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -5228,6 +5645,7 @@
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document Sprint 12 #120
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="20">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Sprint 11</t>
+  </si>
+  <si>
+    <t>Sprint 12</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -361,162 +364,324 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="168">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="182">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2321,8 +2486,90 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="167" headerRowBorderDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="181" headerRowBorderDxfId="180">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="179" totalsRowDxfId="178"/>
+    <tableColumn id="2" name="Min." dataDxfId="177" totalsRowDxfId="176"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="175" totalsRowDxfId="174"/>
+    <tableColumn id="4" name="Total" dataDxfId="173" totalsRowDxfId="172"/>
+    <tableColumn id="5" name="Real" dataDxfId="171" totalsRowDxfId="170"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="169" totalsRowDxfId="168"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B171:G180"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="167" headerRowBorderDxfId="166">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2342,54 +2589,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B157:G166"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="153" headerRowBorderDxfId="152">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2409,9 +2611,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2431,16 +2633,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
     <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
@@ -2453,9 +2648,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
     <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
@@ -2468,9 +2663,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
     <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
@@ -2483,9 +2678,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
     <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
@@ -2498,9 +2693,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
     <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
@@ -2508,21 +2703,6 @@
     <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
     <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2791,10 +2971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G166"/>
+  <dimension ref="B1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="H177" sqref="H177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2805,22 +2985,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -3043,22 +3223,22 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -3277,22 +3457,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
@@ -3511,22 +3691,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -3745,22 +3925,22 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="23"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
@@ -3979,22 +4159,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="22"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
     </row>
     <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
@@ -4213,22 +4393,22 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
     </row>
     <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="23"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
     </row>
     <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
@@ -4447,22 +4627,22 @@
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="22"/>
-      <c r="D99" s="22"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="23"/>
-      <c r="C100" s="23"/>
-      <c r="D100" s="23"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="23"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -4681,22 +4861,22 @@
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="22" t="s">
+      <c r="B113" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="22"/>
-      <c r="G113" s="22"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="23"/>
     </row>
     <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="23"/>
-      <c r="C114" s="23"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="23"/>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
     </row>
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
@@ -4915,22 +5095,22 @@
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="22" t="s">
+      <c r="B127" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="22"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="22"/>
-      <c r="F127" s="22"/>
-      <c r="G127" s="22"/>
+      <c r="C127" s="23"/>
+      <c r="D127" s="23"/>
+      <c r="E127" s="23"/>
+      <c r="F127" s="23"/>
+      <c r="G127" s="23"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="23"/>
-      <c r="C128" s="23"/>
-      <c r="D128" s="23"/>
-      <c r="E128" s="23"/>
-      <c r="F128" s="23"/>
-      <c r="G128" s="23"/>
+      <c r="B128" s="24"/>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="24"/>
     </row>
     <row r="129" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
@@ -5149,22 +5329,22 @@
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="22" t="s">
+      <c r="B141" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C141" s="22"/>
-      <c r="D141" s="22"/>
-      <c r="E141" s="22"/>
-      <c r="F141" s="22"/>
-      <c r="G141" s="22"/>
+      <c r="C141" s="23"/>
+      <c r="D141" s="23"/>
+      <c r="E141" s="23"/>
+      <c r="F141" s="23"/>
+      <c r="G141" s="23"/>
     </row>
     <row r="142" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="23"/>
-      <c r="C142" s="23"/>
-      <c r="D142" s="23"/>
-      <c r="E142" s="23"/>
-      <c r="F142" s="23"/>
-      <c r="G142" s="23"/>
+      <c r="B142" s="24"/>
+      <c r="C142" s="24"/>
+      <c r="D142" s="24"/>
+      <c r="E142" s="24"/>
+      <c r="F142" s="24"/>
+      <c r="G142" s="24"/>
     </row>
     <row r="143" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="5" t="s">
@@ -5383,22 +5563,22 @@
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" s="22" t="s">
+      <c r="B155" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C155" s="22"/>
-      <c r="D155" s="22"/>
-      <c r="E155" s="22"/>
-      <c r="F155" s="22"/>
-      <c r="G155" s="22"/>
+      <c r="C155" s="23"/>
+      <c r="D155" s="23"/>
+      <c r="E155" s="23"/>
+      <c r="F155" s="23"/>
+      <c r="G155" s="23"/>
     </row>
     <row r="156" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="23"/>
-      <c r="C156" s="23"/>
-      <c r="D156" s="23"/>
-      <c r="E156" s="23"/>
-      <c r="F156" s="23"/>
-      <c r="G156" s="23"/>
+      <c r="B156" s="24"/>
+      <c r="C156" s="24"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="24"/>
+      <c r="F156" s="24"/>
+      <c r="G156" s="24"/>
     </row>
     <row r="157" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="s">
@@ -5604,7 +5784,7 @@
       <c r="D166" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E166" s="24">
+      <c r="E166" s="22">
         <f>SUM(E158:E165)/60</f>
         <v>25.75</v>
       </c>
@@ -5616,8 +5796,244 @@
         <v>34</v>
       </c>
     </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B169" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C169" s="23"/>
+      <c r="D169" s="23"/>
+      <c r="E169" s="23"/>
+      <c r="F169" s="23"/>
+      <c r="G169" s="23"/>
+    </row>
+    <row r="170" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="24"/>
+      <c r="C170" s="24"/>
+      <c r="D170" s="24"/>
+      <c r="E170" s="24"/>
+      <c r="F170" s="24"/>
+      <c r="G170" s="24"/>
+    </row>
+    <row r="171" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G171" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B172" s="14">
+        <v>1</v>
+      </c>
+      <c r="C172" s="8">
+        <v>15</v>
+      </c>
+      <c r="D172" s="7">
+        <v>1</v>
+      </c>
+      <c r="E172" s="8">
+        <f>D172*C172</f>
+        <v>15</v>
+      </c>
+      <c r="F172" s="11">
+        <v>2</v>
+      </c>
+      <c r="G172" s="18">
+        <f>F172*C172</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B173" s="15">
+        <v>2</v>
+      </c>
+      <c r="C173" s="10">
+        <v>45</v>
+      </c>
+      <c r="D173" s="9">
+        <v>4</v>
+      </c>
+      <c r="E173" s="10">
+        <f t="shared" ref="E173:E179" si="24">D173*C173</f>
+        <v>180</v>
+      </c>
+      <c r="F173" s="12">
+        <v>3</v>
+      </c>
+      <c r="G173" s="19">
+        <f t="shared" ref="G173:G179" si="25">F173*C173</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B174" s="15">
+        <v>3</v>
+      </c>
+      <c r="C174" s="10">
+        <v>120</v>
+      </c>
+      <c r="D174" s="9">
+        <v>2</v>
+      </c>
+      <c r="E174" s="10">
+        <f t="shared" si="24"/>
+        <v>240</v>
+      </c>
+      <c r="F174" s="12">
+        <v>1</v>
+      </c>
+      <c r="G174" s="19">
+        <f t="shared" si="25"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B175" s="15">
+        <v>5</v>
+      </c>
+      <c r="C175" s="10">
+        <v>300</v>
+      </c>
+      <c r="D175" s="9">
+        <v>1</v>
+      </c>
+      <c r="E175" s="10">
+        <f t="shared" si="24"/>
+        <v>300</v>
+      </c>
+      <c r="F175" s="12">
+        <v>2</v>
+      </c>
+      <c r="G175" s="19">
+        <f t="shared" si="25"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B176" s="15">
+        <v>8</v>
+      </c>
+      <c r="C176" s="10">
+        <v>720</v>
+      </c>
+      <c r="D176" s="9">
+        <v>2</v>
+      </c>
+      <c r="E176" s="10">
+        <f t="shared" si="24"/>
+        <v>1440</v>
+      </c>
+      <c r="F176" s="12">
+        <v>1</v>
+      </c>
+      <c r="G176" s="19">
+        <f t="shared" si="25"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B177" s="15">
+        <v>13</v>
+      </c>
+      <c r="C177" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D177" s="9">
+        <v>0</v>
+      </c>
+      <c r="E177" s="10">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F177" s="12">
+        <v>1</v>
+      </c>
+      <c r="G177" s="19">
+        <f t="shared" si="25"/>
+        <v>1440</v>
+      </c>
+      <c r="H177" s="25"/>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B178" s="15">
+        <v>21</v>
+      </c>
+      <c r="C178" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D178" s="9">
+        <v>0</v>
+      </c>
+      <c r="E178" s="10">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F178" s="12">
+        <v>0</v>
+      </c>
+      <c r="G178" s="19">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="15">
+        <v>40</v>
+      </c>
+      <c r="C179" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D179" s="9">
+        <v>0</v>
+      </c>
+      <c r="E179" s="10">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F179" s="12">
+        <v>0</v>
+      </c>
+      <c r="G179" s="20">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="3"/>
+      <c r="C180" s="16"/>
+      <c r="D180" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E180" s="22">
+        <f>SUM(E172:E179)/60</f>
+        <v>36.25</v>
+      </c>
+      <c r="F180" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G180" s="21">
+        <f>SUM(G172:G179)/60</f>
+        <v>50.75</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B169:G170"/>
     <mergeCell ref="B155:G156"/>
     <mergeCell ref="B141:G142"/>
     <mergeCell ref="B1:G2"/>
@@ -5633,7 +6049,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="12">
+  <tableParts count="13">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -5646,6 +6062,7 @@
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document sprint 13 #127
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Sprint 12</t>
+  </si>
+  <si>
+    <t>Sprint 13</t>
   </si>
 </sst>
 </file>
@@ -367,160 +370,321 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="182">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="196">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2486,8 +2650,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="181" headerRowBorderDxfId="180">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="195" headerRowBorderDxfId="194">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="193" totalsRowDxfId="192"/>
+    <tableColumn id="2" name="Min." dataDxfId="191" totalsRowDxfId="190"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="189" totalsRowDxfId="188"/>
+    <tableColumn id="4" name="Total" dataDxfId="187" totalsRowDxfId="186"/>
+    <tableColumn id="5" name="Real" dataDxfId="185" totalsRowDxfId="184"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="183" totalsRowDxfId="182"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B171:G180"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B185:G194"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="181" headerRowBorderDxfId="180">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2507,69 +2768,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B157:G166"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B171:G180"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="167" headerRowBorderDxfId="166">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="167" headerRowBorderDxfId="166">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2589,9 +2790,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="153" headerRowBorderDxfId="152">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2611,16 +2812,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
     <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
@@ -2633,9 +2827,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
     <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
@@ -2648,9 +2842,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
     <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
@@ -2663,9 +2857,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
     <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
@@ -2678,9 +2872,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
     <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
@@ -2688,21 +2882,6 @@
     <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
     <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2971,10 +3150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H180"/>
+  <dimension ref="B1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="H177" sqref="H177"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="H186" sqref="H186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,22 +3164,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -3223,22 +3402,22 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -3457,22 +3636,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
@@ -3691,22 +3870,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -3925,22 +4104,22 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
@@ -4159,22 +4338,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="23"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="24"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25"/>
     </row>
     <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
@@ -4393,22 +4572,22 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="23" t="s">
+      <c r="B85" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="23"/>
-      <c r="D85" s="23"/>
-      <c r="E85" s="23"/>
-      <c r="F85" s="23"/>
-      <c r="G85" s="23"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
     </row>
     <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="25"/>
     </row>
     <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
@@ -4627,22 +4806,22 @@
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="23" t="s">
+      <c r="B99" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="23"/>
-      <c r="D99" s="23"/>
-      <c r="E99" s="23"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="23"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -4861,22 +5040,22 @@
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="23" t="s">
+      <c r="B113" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
-      <c r="E113" s="23"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="23"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="24"/>
     </row>
     <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
-      <c r="F114" s="24"/>
-      <c r="G114" s="24"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="25"/>
     </row>
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
@@ -5095,22 +5274,22 @@
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="23" t="s">
+      <c r="B127" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="23"/>
-      <c r="D127" s="23"/>
-      <c r="E127" s="23"/>
-      <c r="F127" s="23"/>
-      <c r="G127" s="23"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="24"/>
+      <c r="G127" s="24"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="24"/>
-      <c r="C128" s="24"/>
-      <c r="D128" s="24"/>
-      <c r="E128" s="24"/>
-      <c r="F128" s="24"/>
-      <c r="G128" s="24"/>
+      <c r="B128" s="25"/>
+      <c r="C128" s="25"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="25"/>
+      <c r="F128" s="25"/>
+      <c r="G128" s="25"/>
     </row>
     <row r="129" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
@@ -5329,22 +5508,22 @@
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="23" t="s">
+      <c r="B141" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C141" s="23"/>
-      <c r="D141" s="23"/>
-      <c r="E141" s="23"/>
-      <c r="F141" s="23"/>
-      <c r="G141" s="23"/>
+      <c r="C141" s="24"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="24"/>
+      <c r="F141" s="24"/>
+      <c r="G141" s="24"/>
     </row>
     <row r="142" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="24"/>
-      <c r="C142" s="24"/>
-      <c r="D142" s="24"/>
-      <c r="E142" s="24"/>
-      <c r="F142" s="24"/>
-      <c r="G142" s="24"/>
+      <c r="B142" s="25"/>
+      <c r="C142" s="25"/>
+      <c r="D142" s="25"/>
+      <c r="E142" s="25"/>
+      <c r="F142" s="25"/>
+      <c r="G142" s="25"/>
     </row>
     <row r="143" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="5" t="s">
@@ -5563,22 +5742,22 @@
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" s="23" t="s">
+      <c r="B155" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C155" s="23"/>
-      <c r="D155" s="23"/>
-      <c r="E155" s="23"/>
-      <c r="F155" s="23"/>
-      <c r="G155" s="23"/>
+      <c r="C155" s="24"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="24"/>
+      <c r="F155" s="24"/>
+      <c r="G155" s="24"/>
     </row>
     <row r="156" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="24"/>
-      <c r="C156" s="24"/>
-      <c r="D156" s="24"/>
-      <c r="E156" s="24"/>
-      <c r="F156" s="24"/>
-      <c r="G156" s="24"/>
+      <c r="B156" s="25"/>
+      <c r="C156" s="25"/>
+      <c r="D156" s="25"/>
+      <c r="E156" s="25"/>
+      <c r="F156" s="25"/>
+      <c r="G156" s="25"/>
     </row>
     <row r="157" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="s">
@@ -5797,22 +5976,22 @@
       </c>
     </row>
     <row r="169" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B169" s="23" t="s">
+      <c r="B169" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C169" s="23"/>
-      <c r="D169" s="23"/>
-      <c r="E169" s="23"/>
-      <c r="F169" s="23"/>
-      <c r="G169" s="23"/>
+      <c r="C169" s="24"/>
+      <c r="D169" s="24"/>
+      <c r="E169" s="24"/>
+      <c r="F169" s="24"/>
+      <c r="G169" s="24"/>
     </row>
     <row r="170" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="24"/>
-      <c r="C170" s="24"/>
-      <c r="D170" s="24"/>
-      <c r="E170" s="24"/>
-      <c r="F170" s="24"/>
-      <c r="G170" s="24"/>
+      <c r="B170" s="25"/>
+      <c r="C170" s="25"/>
+      <c r="D170" s="25"/>
+      <c r="E170" s="25"/>
+      <c r="F170" s="25"/>
+      <c r="G170" s="25"/>
     </row>
     <row r="171" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B171" s="5" t="s">
@@ -5965,7 +6144,7 @@
         <f t="shared" si="25"/>
         <v>1440</v>
       </c>
-      <c r="H177" s="25"/>
+      <c r="H177" s="23"/>
     </row>
     <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B178" s="15">
@@ -6031,8 +6210,244 @@
         <v>50.75</v>
       </c>
     </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B183" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C183" s="24"/>
+      <c r="D183" s="24"/>
+      <c r="E183" s="24"/>
+      <c r="F183" s="24"/>
+      <c r="G183" s="24"/>
+    </row>
+    <row r="184" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="25"/>
+      <c r="C184" s="25"/>
+      <c r="D184" s="25"/>
+      <c r="E184" s="25"/>
+      <c r="F184" s="25"/>
+      <c r="G184" s="25"/>
+    </row>
+    <row r="185" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G185" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B186" s="14">
+        <v>1</v>
+      </c>
+      <c r="C186" s="8">
+        <v>15</v>
+      </c>
+      <c r="D186" s="7">
+        <v>1</v>
+      </c>
+      <c r="E186" s="8">
+        <f>D186*C186</f>
+        <v>15</v>
+      </c>
+      <c r="F186" s="11">
+        <v>1</v>
+      </c>
+      <c r="G186" s="18">
+        <f>F186*C186</f>
+        <v>15</v>
+      </c>
+      <c r="H186" s="23"/>
+    </row>
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B187" s="15">
+        <v>2</v>
+      </c>
+      <c r="C187" s="10">
+        <v>45</v>
+      </c>
+      <c r="D187" s="9">
+        <v>0</v>
+      </c>
+      <c r="E187" s="10">
+        <f t="shared" ref="E187:E193" si="26">D187*C187</f>
+        <v>0</v>
+      </c>
+      <c r="F187" s="12">
+        <v>0</v>
+      </c>
+      <c r="G187" s="19">
+        <f t="shared" ref="G187:G193" si="27">F187*C187</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B188" s="15">
+        <v>3</v>
+      </c>
+      <c r="C188" s="10">
+        <v>120</v>
+      </c>
+      <c r="D188" s="9">
+        <v>1</v>
+      </c>
+      <c r="E188" s="10">
+        <f t="shared" si="26"/>
+        <v>120</v>
+      </c>
+      <c r="F188" s="12">
+        <v>1</v>
+      </c>
+      <c r="G188" s="19">
+        <f t="shared" si="27"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B189" s="15">
+        <v>5</v>
+      </c>
+      <c r="C189" s="10">
+        <v>300</v>
+      </c>
+      <c r="D189" s="9">
+        <v>0</v>
+      </c>
+      <c r="E189" s="10">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F189" s="12">
+        <v>0</v>
+      </c>
+      <c r="G189" s="19">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B190" s="15">
+        <v>8</v>
+      </c>
+      <c r="C190" s="10">
+        <v>720</v>
+      </c>
+      <c r="D190" s="9">
+        <v>0</v>
+      </c>
+      <c r="E190" s="10">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F190" s="12">
+        <v>1</v>
+      </c>
+      <c r="G190" s="19">
+        <f t="shared" si="27"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B191" s="15">
+        <v>13</v>
+      </c>
+      <c r="C191" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D191" s="9">
+        <v>1</v>
+      </c>
+      <c r="E191" s="10">
+        <f t="shared" si="26"/>
+        <v>1440</v>
+      </c>
+      <c r="F191" s="12">
+        <v>0</v>
+      </c>
+      <c r="G191" s="19">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B192" s="15">
+        <v>21</v>
+      </c>
+      <c r="C192" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D192" s="9">
+        <v>0</v>
+      </c>
+      <c r="E192" s="10">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F192" s="12">
+        <v>0</v>
+      </c>
+      <c r="G192" s="19">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="15">
+        <v>40</v>
+      </c>
+      <c r="C193" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D193" s="9">
+        <v>0</v>
+      </c>
+      <c r="E193" s="10">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F193" s="12">
+        <v>0</v>
+      </c>
+      <c r="G193" s="20">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="3"/>
+      <c r="C194" s="16"/>
+      <c r="D194" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E194" s="22">
+        <f>SUM(E186:E193)/60</f>
+        <v>26.25</v>
+      </c>
+      <c r="F194" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G194" s="21">
+        <f>SUM(G186:G193)/60</f>
+        <v>14.25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="B183:G184"/>
     <mergeCell ref="B169:G170"/>
     <mergeCell ref="B155:G156"/>
     <mergeCell ref="B141:G142"/>
@@ -6049,7 +6464,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="13">
+  <tableParts count="14">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -6063,6 +6478,7 @@
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document sprint 14 #154
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="22">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -88,11 +88,14 @@
   <si>
     <t>Sprint 13</t>
   </si>
+  <si>
+    <t>Sprint 14</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,149 +384,310 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="196">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="210">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2650,8 +2814,120 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="195" headerRowBorderDxfId="194">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="209" headerRowBorderDxfId="208">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="207" totalsRowDxfId="206"/>
+    <tableColumn id="2" name="Min." dataDxfId="205" totalsRowDxfId="204"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="203" totalsRowDxfId="202"/>
+    <tableColumn id="4" name="Total" dataDxfId="201" totalsRowDxfId="200"/>
+    <tableColumn id="5" name="Real" dataDxfId="199" totalsRowDxfId="198"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="197" totalsRowDxfId="196"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B171:G180"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B185:G194"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B199:G208"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="195" headerRowBorderDxfId="194">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2671,84 +2947,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B157:G166"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B171:G180"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B185:G194"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="181" headerRowBorderDxfId="180">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="181" headerRowBorderDxfId="180">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2768,9 +2969,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="167" headerRowBorderDxfId="166">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="167" headerRowBorderDxfId="166">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2790,16 +2991,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="153" headerRowBorderDxfId="152">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="151" totalsRowDxfId="150"/>
     <tableColumn id="2" name="Min." dataDxfId="149" totalsRowDxfId="148"/>
@@ -2812,9 +3006,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
     <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
@@ -2827,9 +3021,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
     <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
@@ -2842,9 +3036,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
     <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
@@ -2857,9 +3051,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
     <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
@@ -2867,21 +3061,6 @@
     <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
     <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2963,6 +3142,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2998,6 +3194,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3150,10 +3363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H194"/>
+  <dimension ref="B1:H208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="H186" sqref="H186"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="G208" sqref="G208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6445,8 +6658,243 @@
         <v>14.25</v>
       </c>
     </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B197" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C197" s="24"/>
+      <c r="D197" s="24"/>
+      <c r="E197" s="24"/>
+      <c r="F197" s="24"/>
+      <c r="G197" s="24"/>
+    </row>
+    <row r="198" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="25"/>
+      <c r="C198" s="25"/>
+      <c r="D198" s="25"/>
+      <c r="E198" s="25"/>
+      <c r="F198" s="25"/>
+      <c r="G198" s="25"/>
+    </row>
+    <row r="199" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G199" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B200" s="14">
+        <v>1</v>
+      </c>
+      <c r="C200" s="8">
+        <v>15</v>
+      </c>
+      <c r="D200" s="7">
+        <v>1</v>
+      </c>
+      <c r="E200" s="8">
+        <f>D200*C200</f>
+        <v>15</v>
+      </c>
+      <c r="F200" s="11">
+        <v>1</v>
+      </c>
+      <c r="G200" s="18">
+        <f>F200*C200</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B201" s="15">
+        <v>2</v>
+      </c>
+      <c r="C201" s="10">
+        <v>45</v>
+      </c>
+      <c r="D201" s="9">
+        <v>9</v>
+      </c>
+      <c r="E201" s="10">
+        <f t="shared" ref="E201:E207" si="28">D201*C201</f>
+        <v>405</v>
+      </c>
+      <c r="F201" s="12">
+        <v>14</v>
+      </c>
+      <c r="G201" s="19">
+        <f t="shared" ref="G201:G207" si="29">F201*C201</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B202" s="15">
+        <v>3</v>
+      </c>
+      <c r="C202" s="10">
+        <v>120</v>
+      </c>
+      <c r="D202" s="9">
+        <v>9</v>
+      </c>
+      <c r="E202" s="10">
+        <f t="shared" si="28"/>
+        <v>1080</v>
+      </c>
+      <c r="F202" s="12">
+        <v>3</v>
+      </c>
+      <c r="G202" s="19">
+        <f t="shared" si="29"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B203" s="15">
+        <v>5</v>
+      </c>
+      <c r="C203" s="10">
+        <v>300</v>
+      </c>
+      <c r="D203" s="9">
+        <v>2</v>
+      </c>
+      <c r="E203" s="10">
+        <f t="shared" si="28"/>
+        <v>600</v>
+      </c>
+      <c r="F203" s="12">
+        <v>3</v>
+      </c>
+      <c r="G203" s="19">
+        <f t="shared" si="29"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B204" s="15">
+        <v>8</v>
+      </c>
+      <c r="C204" s="10">
+        <v>720</v>
+      </c>
+      <c r="D204" s="9">
+        <v>7</v>
+      </c>
+      <c r="E204" s="10">
+        <f t="shared" si="28"/>
+        <v>5040</v>
+      </c>
+      <c r="F204" s="12">
+        <v>6</v>
+      </c>
+      <c r="G204" s="19">
+        <f t="shared" si="29"/>
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B205" s="15">
+        <v>13</v>
+      </c>
+      <c r="C205" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D205" s="9">
+        <v>1</v>
+      </c>
+      <c r="E205" s="10">
+        <f t="shared" si="28"/>
+        <v>1440</v>
+      </c>
+      <c r="F205" s="12">
+        <v>1</v>
+      </c>
+      <c r="G205" s="19">
+        <f t="shared" si="29"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B206" s="15">
+        <v>21</v>
+      </c>
+      <c r="C206" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D206" s="9">
+        <v>0</v>
+      </c>
+      <c r="E206" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="F206" s="12">
+        <v>1</v>
+      </c>
+      <c r="G206" s="19">
+        <f t="shared" si="29"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="15">
+        <v>40</v>
+      </c>
+      <c r="C207" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D207" s="9">
+        <v>0</v>
+      </c>
+      <c r="E207" s="10">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="F207" s="12">
+        <v>0</v>
+      </c>
+      <c r="G207" s="20">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="3"/>
+      <c r="C208" s="16"/>
+      <c r="D208" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E208" s="22">
+        <f>SUM(E200:E207)/60</f>
+        <v>143</v>
+      </c>
+      <c r="F208" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G208" s="21">
+        <f>SUM(G200:G207)/60</f>
+        <v>187.75</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="B197:G198"/>
     <mergeCell ref="B183:G184"/>
     <mergeCell ref="B169:G170"/>
     <mergeCell ref="B155:G156"/>
@@ -6464,7 +6912,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="14">
+  <tableParts count="15">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -6479,6 +6927,7 @@
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document sprint 15 #162
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="23">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Sprint 14</t>
+  </si>
+  <si>
+    <t>Sprint 15</t>
   </si>
 </sst>
 </file>
@@ -384,149 +387,310 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="210">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="224">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2814,8 +2978,135 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="209" headerRowBorderDxfId="208">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="223" headerRowBorderDxfId="222">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="221" totalsRowDxfId="220"/>
+    <tableColumn id="2" name="Min." dataDxfId="219" totalsRowDxfId="218"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="217" totalsRowDxfId="216"/>
+    <tableColumn id="4" name="Total" dataDxfId="215" totalsRowDxfId="214"/>
+    <tableColumn id="5" name="Real" dataDxfId="213" totalsRowDxfId="212"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="211" totalsRowDxfId="210"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B171:G180"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B185:G194"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B199:G208"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla181011234567121314151617" displayName="Tabla181011234567121314151617" ref="B213:G222" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B213:G222"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="209" headerRowBorderDxfId="208">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2835,99 +3126,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B157:G166"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B171:G180"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B185:G194"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B199:G208"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="195" headerRowBorderDxfId="194">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="195" headerRowBorderDxfId="194">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2947,9 +3148,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="181" headerRowBorderDxfId="180">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="181" headerRowBorderDxfId="180">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2969,16 +3170,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="167" headerRowBorderDxfId="166">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="167" headerRowBorderDxfId="166">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="165" totalsRowDxfId="164"/>
     <tableColumn id="2" name="Min." dataDxfId="163" totalsRowDxfId="162"/>
@@ -2991,9 +3185,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="153" headerRowBorderDxfId="152">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="151" totalsRowDxfId="150"/>
     <tableColumn id="2" name="Min." dataDxfId="149" totalsRowDxfId="148"/>
@@ -3006,9 +3200,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
     <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
@@ -3021,9 +3215,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
     <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
@@ -3036,9 +3230,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
     <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
@@ -3046,21 +3240,6 @@
     <tableColumn id="4" name="Total" dataDxfId="103" totalsRowDxfId="102"/>
     <tableColumn id="5" name="Real" dataDxfId="101" totalsRowDxfId="100"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="99" totalsRowDxfId="98"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -3363,10 +3542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H208"/>
+  <dimension ref="B1:H222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="G208" sqref="G208"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="G222" sqref="G222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6892,27 +7071,262 @@
         <v>187.75</v>
       </c>
     </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B211" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C211" s="24"/>
+      <c r="D211" s="24"/>
+      <c r="E211" s="24"/>
+      <c r="F211" s="24"/>
+      <c r="G211" s="24"/>
+    </row>
+    <row r="212" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="25"/>
+      <c r="C212" s="25"/>
+      <c r="D212" s="25"/>
+      <c r="E212" s="25"/>
+      <c r="F212" s="25"/>
+      <c r="G212" s="25"/>
+    </row>
+    <row r="213" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B213" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G213" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B214" s="14">
+        <v>1</v>
+      </c>
+      <c r="C214" s="8">
+        <v>15</v>
+      </c>
+      <c r="D214" s="7">
+        <v>2</v>
+      </c>
+      <c r="E214" s="8">
+        <f>D214*C214</f>
+        <v>30</v>
+      </c>
+      <c r="F214" s="11">
+        <v>2</v>
+      </c>
+      <c r="G214" s="18">
+        <f>F214*C214</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B215" s="15">
+        <v>2</v>
+      </c>
+      <c r="C215" s="10">
+        <v>45</v>
+      </c>
+      <c r="D215" s="9">
+        <v>2</v>
+      </c>
+      <c r="E215" s="10">
+        <f t="shared" ref="E215:E221" si="30">D215*C215</f>
+        <v>90</v>
+      </c>
+      <c r="F215" s="12">
+        <v>3</v>
+      </c>
+      <c r="G215" s="19">
+        <f t="shared" ref="G215:G221" si="31">F215*C215</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B216" s="15">
+        <v>3</v>
+      </c>
+      <c r="C216" s="10">
+        <v>120</v>
+      </c>
+      <c r="D216" s="9">
+        <v>5</v>
+      </c>
+      <c r="E216" s="10">
+        <f t="shared" si="30"/>
+        <v>600</v>
+      </c>
+      <c r="F216" s="12">
+        <v>3</v>
+      </c>
+      <c r="G216" s="19">
+        <f t="shared" si="31"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B217" s="15">
+        <v>5</v>
+      </c>
+      <c r="C217" s="10">
+        <v>300</v>
+      </c>
+      <c r="D217" s="9">
+        <v>3</v>
+      </c>
+      <c r="E217" s="10">
+        <f t="shared" si="30"/>
+        <v>900</v>
+      </c>
+      <c r="F217" s="12">
+        <v>1</v>
+      </c>
+      <c r="G217" s="19">
+        <f t="shared" si="31"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B218" s="15">
+        <v>8</v>
+      </c>
+      <c r="C218" s="10">
+        <v>720</v>
+      </c>
+      <c r="D218" s="9">
+        <v>1</v>
+      </c>
+      <c r="E218" s="10">
+        <f t="shared" si="30"/>
+        <v>720</v>
+      </c>
+      <c r="F218" s="12">
+        <v>2</v>
+      </c>
+      <c r="G218" s="19">
+        <f t="shared" si="31"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B219" s="15">
+        <v>13</v>
+      </c>
+      <c r="C219" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D219" s="9">
+        <v>0</v>
+      </c>
+      <c r="E219" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="F219" s="12">
+        <v>0</v>
+      </c>
+      <c r="G219" s="19">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B220" s="15">
+        <v>21</v>
+      </c>
+      <c r="C220" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D220" s="9">
+        <v>0</v>
+      </c>
+      <c r="E220" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="F220" s="12">
+        <v>0</v>
+      </c>
+      <c r="G220" s="19">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B221" s="15">
+        <v>40</v>
+      </c>
+      <c r="C221" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D221" s="9">
+        <v>0</v>
+      </c>
+      <c r="E221" s="10">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="F221" s="12">
+        <v>0</v>
+      </c>
+      <c r="G221" s="20">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B222" s="3"/>
+      <c r="C222" s="16"/>
+      <c r="D222" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E222" s="22">
+        <f>SUM(E214:E221)/60</f>
+        <v>39</v>
+      </c>
+      <c r="F222" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G222" s="21">
+        <f>SUM(G214:G221)/60</f>
+        <v>37.75</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B211:G212"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B113:G114"/>
+    <mergeCell ref="B99:G100"/>
+    <mergeCell ref="B71:G72"/>
+    <mergeCell ref="B85:G86"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="B57:G58"/>
     <mergeCell ref="B197:G198"/>
     <mergeCell ref="B183:G184"/>
     <mergeCell ref="B169:G170"/>
     <mergeCell ref="B155:G156"/>
     <mergeCell ref="B141:G142"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="B29:G30"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="B57:G58"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B113:G114"/>
-    <mergeCell ref="B99:G100"/>
-    <mergeCell ref="B71:G72"/>
-    <mergeCell ref="B85:G86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="15">
+  <tableParts count="16">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -6928,6 +7342,7 @@
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix exclusions sonarqube #155
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="25">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -94,12 +94,18 @@
   <si>
     <t>Sprint 15</t>
   </si>
+  <si>
+    <t>Total horas estimadas</t>
+  </si>
+  <si>
+    <t>Total horas reales</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +151,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +184,18 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -312,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -383,6 +416,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,146 +429,146 @@
   <dxfs count="224">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3093,12 +3132,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla181011234567121314151617" displayName="Tabla181011234567121314151617" ref="B213:G222" headerRowDxfId="13" headerRowBorderDxfId="12">
   <autoFilter ref="B213:G222"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" name="Min." dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Total" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Real" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -3542,10 +3581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H222"/>
+  <dimension ref="B1:J222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="G222" sqref="G222"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3553,9 +3592,10 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
         <v>2</v>
       </c>
@@ -3565,7 +3605,7 @@
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -3573,7 +3613,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3592,8 +3632,15 @@
       <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="27">
+        <f>E12+E26+E40+E54+E68+E82+E96+E110+E124+E138+E152+E166+E180+E194+E208+E222</f>
+        <v>521.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
         <v>1</v>
       </c>
@@ -3614,8 +3661,15 @@
         <f>F4*C4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="27">
+        <f>G12+G40+G54+G68+G82+G96+G110+G124+G138+G152+G166+G180+G194+G208+G222</f>
+        <v>651.75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="15">
         <v>2</v>
       </c>
@@ -3637,7 +3691,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="15">
         <v>3</v>
       </c>
@@ -3659,7 +3713,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
         <v>5</v>
       </c>
@@ -3681,7 +3735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="15">
         <v>8</v>
       </c>
@@ -3703,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
         <v>13</v>
       </c>
@@ -3725,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="15">
         <v>21</v>
       </c>
@@ -3748,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15">
         <v>40</v>
       </c>
@@ -3771,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="6" t="s">
@@ -3789,11 +3843,11 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
         <v>4</v>
       </c>
@@ -3803,7 +3857,7 @@
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
@@ -7307,17 +7361,17 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="B57:G58"/>
     <mergeCell ref="B211:G212"/>
     <mergeCell ref="B127:G128"/>
     <mergeCell ref="B113:G114"/>
     <mergeCell ref="B99:G100"/>
     <mergeCell ref="B71:G72"/>
     <mergeCell ref="B85:G86"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="B29:G30"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="B57:G58"/>
     <mergeCell ref="B197:G198"/>
     <mergeCell ref="B183:G184"/>
     <mergeCell ref="B169:G170"/>

</xml_diff>

<commit_message>
Document Sprint 16 #177
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="26">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Total horas reales</t>
+  </si>
+  <si>
+    <t>Sprint 16</t>
   </si>
 </sst>
 </file>
@@ -410,23 +413,184 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="224">
+  <dxfs count="238">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -3017,8 +3181,150 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="223" headerRowBorderDxfId="222">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="237" headerRowBorderDxfId="236">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="235" totalsRowDxfId="234"/>
+    <tableColumn id="2" name="Min." dataDxfId="233" totalsRowDxfId="232"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="231" totalsRowDxfId="230"/>
+    <tableColumn id="4" name="Total" dataDxfId="229" totalsRowDxfId="228"/>
+    <tableColumn id="5" name="Real" dataDxfId="227" totalsRowDxfId="226"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="225" totalsRowDxfId="224"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
+    <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="4" name="Total" dataDxfId="103" totalsRowDxfId="102"/>
+    <tableColumn id="5" name="Real" dataDxfId="101" totalsRowDxfId="100"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="99" totalsRowDxfId="98"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B171:G180"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B185:G194"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B199:G208"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla181011234567121314151617" displayName="Tabla181011234567121314151617" ref="B213:G222" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B213:G222"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla18101123456712131415161718" displayName="Tabla18101123456712131415161718" ref="B227:G236" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B227:G236"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="223" headerRowBorderDxfId="222">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3038,114 +3344,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B157:G166"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B171:G180"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B185:G194"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B199:G208"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla181011234567121314151617" displayName="Tabla181011234567121314151617" ref="B213:G222" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B213:G222"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="2" name="Min." dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Total" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="5" name="Real" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="209" headerRowBorderDxfId="208">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="209" headerRowBorderDxfId="208">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3165,9 +3366,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="195" headerRowBorderDxfId="194">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="195" headerRowBorderDxfId="194">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3187,16 +3388,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="181" headerRowBorderDxfId="180">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="181" headerRowBorderDxfId="180">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="179" totalsRowDxfId="178"/>
     <tableColumn id="2" name="Min." dataDxfId="177" totalsRowDxfId="176"/>
@@ -3209,9 +3403,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="167" headerRowBorderDxfId="166">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="167" headerRowBorderDxfId="166">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="165" totalsRowDxfId="164"/>
     <tableColumn id="2" name="Min." dataDxfId="163" totalsRowDxfId="162"/>
@@ -3224,9 +3418,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="153" headerRowBorderDxfId="152">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="151" totalsRowDxfId="150"/>
     <tableColumn id="2" name="Min." dataDxfId="149" totalsRowDxfId="148"/>
@@ -3239,9 +3433,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
     <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
@@ -3254,9 +3448,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
     <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
@@ -3264,21 +3458,6 @@
     <tableColumn id="4" name="Total" dataDxfId="117" totalsRowDxfId="116"/>
     <tableColumn id="5" name="Real" dataDxfId="115" totalsRowDxfId="114"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
-    <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="105" totalsRowDxfId="104"/>
-    <tableColumn id="4" name="Total" dataDxfId="103" totalsRowDxfId="102"/>
-    <tableColumn id="5" name="Real" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="99" totalsRowDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -3581,10 +3760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J222"/>
+  <dimension ref="B1:J236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,22 +3775,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -3632,12 +3811,12 @@
       <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="27">
-        <f>E12+E26+E40+E54+E68+E82+E96+E110+E124+E138+E152+E166+E180+E194+E208+E222</f>
-        <v>521.5</v>
+      <c r="J3" s="25">
+        <f>E12+E26+E40+E54+E68+E82+E96+E110+E124+E138+E152+E166+E180+E194+E208+E222+E236</f>
+        <v>567.25</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3661,12 +3840,12 @@
         <f>F4*C4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="27">
-        <f>G12+G40+G54+G68+G82+G96+G110+G124+G138+G152+G166+G180+G194+G208+G222</f>
-        <v>651.75</v>
+      <c r="J4" s="25">
+        <f>G12+G40+G54+G68+G82+G96+G110+G124+G138+G152+G166+G180+G194+G208+G222+G236</f>
+        <v>697</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -3848,22 +4027,22 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -4082,22 +4261,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
@@ -4316,22 +4495,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -4550,22 +4729,22 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
@@ -4784,22 +4963,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
@@ -5018,22 +5197,22 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="26"/>
+      <c r="G85" s="26"/>
     </row>
     <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="27"/>
     </row>
     <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
@@ -5252,22 +5431,22 @@
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="24"/>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
-      <c r="G99" s="24"/>
+      <c r="C99" s="26"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="26"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -5486,22 +5665,22 @@
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="24" t="s">
+      <c r="B113" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="24"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="24"/>
+      <c r="C113" s="26"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26"/>
+      <c r="G113" s="26"/>
     </row>
     <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="25"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="25"/>
-      <c r="G114" s="25"/>
+      <c r="B114" s="27"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
+      <c r="G114" s="27"/>
     </row>
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
@@ -5720,22 +5899,22 @@
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="24" t="s">
+      <c r="B127" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="24"/>
-      <c r="D127" s="24"/>
-      <c r="E127" s="24"/>
-      <c r="F127" s="24"/>
-      <c r="G127" s="24"/>
+      <c r="C127" s="26"/>
+      <c r="D127" s="26"/>
+      <c r="E127" s="26"/>
+      <c r="F127" s="26"/>
+      <c r="G127" s="26"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="25"/>
-      <c r="C128" s="25"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="25"/>
-      <c r="G128" s="25"/>
+      <c r="B128" s="27"/>
+      <c r="C128" s="27"/>
+      <c r="D128" s="27"/>
+      <c r="E128" s="27"/>
+      <c r="F128" s="27"/>
+      <c r="G128" s="27"/>
     </row>
     <row r="129" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
@@ -5954,22 +6133,22 @@
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="24" t="s">
+      <c r="B141" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C141" s="24"/>
-      <c r="D141" s="24"/>
-      <c r="E141" s="24"/>
-      <c r="F141" s="24"/>
-      <c r="G141" s="24"/>
+      <c r="C141" s="26"/>
+      <c r="D141" s="26"/>
+      <c r="E141" s="26"/>
+      <c r="F141" s="26"/>
+      <c r="G141" s="26"/>
     </row>
     <row r="142" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="25"/>
-      <c r="C142" s="25"/>
-      <c r="D142" s="25"/>
-      <c r="E142" s="25"/>
-      <c r="F142" s="25"/>
-      <c r="G142" s="25"/>
+      <c r="B142" s="27"/>
+      <c r="C142" s="27"/>
+      <c r="D142" s="27"/>
+      <c r="E142" s="27"/>
+      <c r="F142" s="27"/>
+      <c r="G142" s="27"/>
     </row>
     <row r="143" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="5" t="s">
@@ -6188,22 +6367,22 @@
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" s="24" t="s">
+      <c r="B155" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C155" s="24"/>
-      <c r="D155" s="24"/>
-      <c r="E155" s="24"/>
-      <c r="F155" s="24"/>
-      <c r="G155" s="24"/>
+      <c r="C155" s="26"/>
+      <c r="D155" s="26"/>
+      <c r="E155" s="26"/>
+      <c r="F155" s="26"/>
+      <c r="G155" s="26"/>
     </row>
     <row r="156" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="25"/>
-      <c r="C156" s="25"/>
-      <c r="D156" s="25"/>
-      <c r="E156" s="25"/>
-      <c r="F156" s="25"/>
-      <c r="G156" s="25"/>
+      <c r="B156" s="27"/>
+      <c r="C156" s="27"/>
+      <c r="D156" s="27"/>
+      <c r="E156" s="27"/>
+      <c r="F156" s="27"/>
+      <c r="G156" s="27"/>
     </row>
     <row r="157" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="s">
@@ -6422,22 +6601,22 @@
       </c>
     </row>
     <row r="169" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B169" s="24" t="s">
+      <c r="B169" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C169" s="24"/>
-      <c r="D169" s="24"/>
-      <c r="E169" s="24"/>
-      <c r="F169" s="24"/>
-      <c r="G169" s="24"/>
+      <c r="C169" s="26"/>
+      <c r="D169" s="26"/>
+      <c r="E169" s="26"/>
+      <c r="F169" s="26"/>
+      <c r="G169" s="26"/>
     </row>
     <row r="170" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="25"/>
-      <c r="C170" s="25"/>
-      <c r="D170" s="25"/>
-      <c r="E170" s="25"/>
-      <c r="F170" s="25"/>
-      <c r="G170" s="25"/>
+      <c r="B170" s="27"/>
+      <c r="C170" s="27"/>
+      <c r="D170" s="27"/>
+      <c r="E170" s="27"/>
+      <c r="F170" s="27"/>
+      <c r="G170" s="27"/>
     </row>
     <row r="171" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B171" s="5" t="s">
@@ -6657,22 +6836,22 @@
       </c>
     </row>
     <row r="183" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B183" s="24" t="s">
+      <c r="B183" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C183" s="24"/>
-      <c r="D183" s="24"/>
-      <c r="E183" s="24"/>
-      <c r="F183" s="24"/>
-      <c r="G183" s="24"/>
+      <c r="C183" s="26"/>
+      <c r="D183" s="26"/>
+      <c r="E183" s="26"/>
+      <c r="F183" s="26"/>
+      <c r="G183" s="26"/>
     </row>
     <row r="184" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B184" s="25"/>
-      <c r="C184" s="25"/>
-      <c r="D184" s="25"/>
-      <c r="E184" s="25"/>
-      <c r="F184" s="25"/>
-      <c r="G184" s="25"/>
+      <c r="B184" s="27"/>
+      <c r="C184" s="27"/>
+      <c r="D184" s="27"/>
+      <c r="E184" s="27"/>
+      <c r="F184" s="27"/>
+      <c r="G184" s="27"/>
     </row>
     <row r="185" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B185" s="5" t="s">
@@ -6892,22 +7071,22 @@
       </c>
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B197" s="24" t="s">
+      <c r="B197" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C197" s="24"/>
-      <c r="D197" s="24"/>
-      <c r="E197" s="24"/>
-      <c r="F197" s="24"/>
-      <c r="G197" s="24"/>
+      <c r="C197" s="26"/>
+      <c r="D197" s="26"/>
+      <c r="E197" s="26"/>
+      <c r="F197" s="26"/>
+      <c r="G197" s="26"/>
     </row>
     <row r="198" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="25"/>
-      <c r="C198" s="25"/>
-      <c r="D198" s="25"/>
-      <c r="E198" s="25"/>
-      <c r="F198" s="25"/>
-      <c r="G198" s="25"/>
+      <c r="B198" s="27"/>
+      <c r="C198" s="27"/>
+      <c r="D198" s="27"/>
+      <c r="E198" s="27"/>
+      <c r="F198" s="27"/>
+      <c r="G198" s="27"/>
     </row>
     <row r="199" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B199" s="5" t="s">
@@ -7126,22 +7305,22 @@
       </c>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B211" s="24" t="s">
+      <c r="B211" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C211" s="24"/>
-      <c r="D211" s="24"/>
-      <c r="E211" s="24"/>
-      <c r="F211" s="24"/>
-      <c r="G211" s="24"/>
+      <c r="C211" s="26"/>
+      <c r="D211" s="26"/>
+      <c r="E211" s="26"/>
+      <c r="F211" s="26"/>
+      <c r="G211" s="26"/>
     </row>
     <row r="212" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B212" s="25"/>
-      <c r="C212" s="25"/>
-      <c r="D212" s="25"/>
-      <c r="E212" s="25"/>
-      <c r="F212" s="25"/>
-      <c r="G212" s="25"/>
+      <c r="B212" s="27"/>
+      <c r="C212" s="27"/>
+      <c r="D212" s="27"/>
+      <c r="E212" s="27"/>
+      <c r="F212" s="27"/>
+      <c r="G212" s="27"/>
     </row>
     <row r="213" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B213" s="5" t="s">
@@ -7359,13 +7538,243 @@
         <v>37.75</v>
       </c>
     </row>
+    <row r="225" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B225" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C225" s="26"/>
+      <c r="D225" s="26"/>
+      <c r="E225" s="26"/>
+      <c r="F225" s="26"/>
+      <c r="G225" s="26"/>
+    </row>
+    <row r="226" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B226" s="27"/>
+      <c r="C226" s="27"/>
+      <c r="D226" s="27"/>
+      <c r="E226" s="27"/>
+      <c r="F226" s="27"/>
+      <c r="G226" s="27"/>
+    </row>
+    <row r="227" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B227" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G227" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B228" s="14">
+        <v>1</v>
+      </c>
+      <c r="C228" s="8">
+        <v>15</v>
+      </c>
+      <c r="D228" s="7">
+        <v>3</v>
+      </c>
+      <c r="E228" s="8">
+        <f>D228*C228</f>
+        <v>45</v>
+      </c>
+      <c r="F228" s="11">
+        <v>4</v>
+      </c>
+      <c r="G228" s="18">
+        <f>F228*C228</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="229" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B229" s="15">
+        <v>2</v>
+      </c>
+      <c r="C229" s="10">
+        <v>45</v>
+      </c>
+      <c r="D229" s="9">
+        <v>4</v>
+      </c>
+      <c r="E229" s="10">
+        <f t="shared" ref="E229:E235" si="32">D229*C229</f>
+        <v>180</v>
+      </c>
+      <c r="F229" s="12">
+        <v>3</v>
+      </c>
+      <c r="G229" s="19">
+        <f t="shared" ref="G229:G235" si="33">F229*C229</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="230" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B230" s="15">
+        <v>3</v>
+      </c>
+      <c r="C230" s="10">
+        <v>120</v>
+      </c>
+      <c r="D230" s="9">
+        <v>5</v>
+      </c>
+      <c r="E230" s="10">
+        <f t="shared" si="32"/>
+        <v>600</v>
+      </c>
+      <c r="F230" s="12">
+        <v>5</v>
+      </c>
+      <c r="G230" s="19">
+        <f t="shared" si="33"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="231" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B231" s="15">
+        <v>5</v>
+      </c>
+      <c r="C231" s="10">
+        <v>300</v>
+      </c>
+      <c r="D231" s="9">
+        <v>4</v>
+      </c>
+      <c r="E231" s="10">
+        <f t="shared" si="32"/>
+        <v>1200</v>
+      </c>
+      <c r="F231" s="12">
+        <v>4</v>
+      </c>
+      <c r="G231" s="19">
+        <f t="shared" si="33"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="232" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B232" s="15">
+        <v>8</v>
+      </c>
+      <c r="C232" s="10">
+        <v>720</v>
+      </c>
+      <c r="D232" s="9">
+        <v>1</v>
+      </c>
+      <c r="E232" s="10">
+        <f t="shared" si="32"/>
+        <v>720</v>
+      </c>
+      <c r="F232" s="12">
+        <v>1</v>
+      </c>
+      <c r="G232" s="19">
+        <f t="shared" si="33"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="233" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B233" s="15">
+        <v>13</v>
+      </c>
+      <c r="C233" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D233" s="9">
+        <v>0</v>
+      </c>
+      <c r="E233" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="F233" s="12">
+        <v>0</v>
+      </c>
+      <c r="G233" s="19">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B234" s="15">
+        <v>21</v>
+      </c>
+      <c r="C234" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D234" s="9">
+        <v>0</v>
+      </c>
+      <c r="E234" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="F234" s="12">
+        <v>0</v>
+      </c>
+      <c r="G234" s="19">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B235" s="15">
+        <v>40</v>
+      </c>
+      <c r="C235" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D235" s="9">
+        <v>0</v>
+      </c>
+      <c r="E235" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="F235" s="12">
+        <v>0</v>
+      </c>
+      <c r="G235" s="20">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B236" s="3"/>
+      <c r="C236" s="16"/>
+      <c r="D236" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E236" s="22">
+        <f>SUM(E228:E235)/60</f>
+        <v>45.75</v>
+      </c>
+      <c r="F236" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G236" s="21">
+        <f>SUM(G228:G235)/60</f>
+        <v>45.25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="B29:G30"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="B57:G58"/>
+  <mergeCells count="17">
+    <mergeCell ref="B225:G226"/>
     <mergeCell ref="B211:G212"/>
     <mergeCell ref="B127:G128"/>
     <mergeCell ref="B113:G114"/>
@@ -7377,10 +7786,15 @@
     <mergeCell ref="B169:G170"/>
     <mergeCell ref="B155:G156"/>
     <mergeCell ref="B141:G142"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="B57:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="16">
+  <tableParts count="17">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -7397,6 +7811,7 @@
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>